<commit_message>
li xiang L6 added
</commit_message>
<xml_diff>
--- a/public/assets/docs/byd_han_ev.xlsx
+++ b/public/assets/docs/byd_han_ev.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamoliddin\Desktop\DriveDeals\public\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208EBC38-75E1-4A32-BD80-5E67E97707A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE334B31-D7DB-4942-BC93-AB8D27FF40A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +453,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -524,54 +531,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Oddiy" xfId="0" builtinId="0"/>
+    <cellStyle name="Oddiy 2" xfId="1" xr:uid="{FC2C4A56-3BEA-43C4-9E56-5E9BDD0A8399}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -849,1329 +847,1300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="57.1">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="57.1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.55">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" ht="28.55">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>2024</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>2024</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>2024</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="28.55">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="28.55">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="71.349999999999994">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="71.349999999999994">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="85.6">
-      <c r="A8" s="3" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="85.6">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" ht="42.8">
-      <c r="A9" s="3" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="42.8">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="114.15">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="114.15">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="28.55">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="28.55">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="71.349999999999994">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="71.349999999999994">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.55">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="28.55">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" ht="57.1">
-      <c r="A15" s="3" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="57.1">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" ht="42.8">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="42.8">
+      <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.55">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:5" ht="28.55">
+      <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="71.349999999999994">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:5" ht="71.349999999999994">
+      <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" ht="71.349999999999994">
-      <c r="A20" s="3" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="71.349999999999994">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" ht="71.349999999999994">
-      <c r="A21" s="3" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="71.349999999999994">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="99.85">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="99.85">
+      <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="9" t="s">
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.55">
-      <c r="A24" s="3" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.55">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" ht="28.55">
-      <c r="A25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="28.55">
+      <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" ht="28.55">
-      <c r="A26" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.55">
+      <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" ht="57.1">
-      <c r="A27" s="3" t="s">
+      <c r="E26" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57.1">
+      <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" ht="71.349999999999994">
-      <c r="A28" s="3" t="s">
+      <c r="B27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="71.349999999999994">
+      <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="42.8">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:5" ht="42.8">
+      <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" ht="99.85">
-      <c r="A30" s="3" t="s">
+      <c r="B29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="99.85">
+      <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" ht="28.55">
-      <c r="A31" s="3" t="s">
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.55">
+      <c r="A31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" ht="57.1">
-      <c r="A32" s="3" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="57.1">
+      <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:5" ht="71.349999999999994">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="99.85">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="99.85">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="57.1">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="71.349999999999994">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="B37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="42.8">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="42.8">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="B39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="71.349999999999994">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="85.6">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="B41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="85.6">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="B42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="128.4">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="B43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="128.4">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="B44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="85.6">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="5" t="s">
+      <c r="B45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="57.1">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="B46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="85.6">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="71.349999999999994">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" s="5" t="s">
+      <c r="B48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="99.85">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="B49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="99.85">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="85.6">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="5" t="s">
+      <c r="B51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="99.85">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="B52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="57.1">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="B53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="99.85">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="B54" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="57.1">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="114.15">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="85.6">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="128.4">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="3">
         <v>15.6</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C58" s="3">
         <v>15.6</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="3">
         <v>15.6</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="3">
         <v>15.6</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="57.1">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="3">
         <v>12.3</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="3">
         <v>12.3</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="3">
         <v>12.3</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="3">
         <v>12.3</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="28.55">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E60" s="5" t="s">
+      <c r="C60" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="57.1">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E61" s="5" t="s">
+      <c r="B61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="42.8">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E62" s="5" t="s">
+      <c r="B62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="28.55">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E63" s="5" t="s">
+      <c r="B63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="85.6">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E64" s="5" t="s">
+      <c r="B64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="71.349999999999994">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E65" s="5" t="s">
+      <c r="B65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="85.6">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E66" s="5" t="s">
+      <c r="B66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="57.1">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E67" s="5" t="s">
+      <c r="B67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="71.349999999999994">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E68" s="5" t="s">
+      <c r="B68" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="57.1">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E69" s="5" t="s">
+      <c r="B69" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="71.349999999999994">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="114.15">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E71" s="5" t="s">
+      <c r="B71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="57.1">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E72" s="5" t="s">
+      <c r="B72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="28.55">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="85.6">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="99.85">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="57.1">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E77" s="5" t="s">
+      <c r="B77" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="99.85">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="12"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A73:E73"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A73:E73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>